<commit_message>
fixed some data files, added python scripts for figures 1 and 4
</commit_message>
<xml_diff>
--- a/Data/Auranofin/MotorBehaviordata_Auranofin_Livia_010924.xlsx
+++ b/Data/Auranofin/MotorBehaviordata_Auranofin_Livia_010924.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livia\Documents\Data Mito\data\raw\Auranofin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiaoguienko/git/LHMorais2024/Data/Auranofin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7C377E-0440-4223-8E82-B079CCAACF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BA843D-30A4-4141-A1CF-A57F98AC928F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{14CC993E-0CDB-4C1F-BA41-A215F3DE6160}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{14CC993E-0CDB-4C1F-BA41-A215F3DE6160}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="41">
   <si>
     <t>Pole_T1</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT </t>
   </si>
   <si>
     <t>V</t>
@@ -529,28 +526,28 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -570,7 +567,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -578,32 +575,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -611,7 +608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -628,16 +625,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6AB8CE-CDE7-4CC0-B7A8-69D07539B035}">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="89" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:M49"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -645,7 +642,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>30</v>
@@ -663,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -678,7 +675,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>22122</v>
       </c>
@@ -686,13 +683,13 @@
         <v>5203</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <v>7.38</v>
@@ -719,7 +716,7 @@
         <v>9.0533333333333328</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>22122</v>
       </c>
@@ -727,13 +724,13 @@
         <v>5204</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <v>10.58</v>
@@ -760,7 +757,7 @@
         <v>6.8500000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>22122</v>
       </c>
@@ -768,13 +765,13 @@
         <v>5207</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <v>7.33</v>
@@ -801,7 +798,7 @@
         <v>4.3299999999999992</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>22122</v>
       </c>
@@ -809,13 +806,13 @@
         <v>5208</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>8.32</v>
@@ -842,7 +839,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>22122</v>
       </c>
@@ -850,13 +847,13 @@
         <v>5209</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6">
         <v>16.329999999999998</v>
@@ -883,7 +880,7 @@
         <v>12.973333333333334</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>22122</v>
       </c>
@@ -891,13 +888,13 @@
         <v>5210</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7">
         <v>12.71</v>
@@ -924,7 +921,7 @@
         <v>13.74</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>22122</v>
       </c>
@@ -932,13 +929,13 @@
         <v>5211</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <v>7.28</v>
@@ -965,7 +962,7 @@
         <v>6.5766666666666671</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>22122</v>
       </c>
@@ -973,13 +970,13 @@
         <v>5199</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>3.7</v>
@@ -1006,7 +1003,7 @@
         <v>7.5333333333333323</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>22122</v>
       </c>
@@ -1014,13 +1011,13 @@
         <v>5200</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>9.57</v>
@@ -1047,7 +1044,7 @@
         <v>4.1499999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>22122</v>
       </c>
@@ -1055,13 +1052,13 @@
         <v>5201</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11">
         <v>5.45</v>
@@ -1088,7 +1085,7 @@
         <v>14.443333333333333</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>22122</v>
       </c>
@@ -1096,13 +1093,13 @@
         <v>5230</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12">
         <v>14.7</v>
@@ -1129,7 +1126,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>22122</v>
       </c>
@@ -1137,13 +1134,13 @@
         <v>5231</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13">
         <v>22.96</v>
@@ -1170,7 +1167,7 @@
         <v>9.0233333333333334</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>22122</v>
       </c>
@@ -1178,13 +1175,13 @@
         <v>5232</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14">
         <v>19.399999999999999</v>
@@ -1211,7 +1208,7 @@
         <v>3.4633333333333334</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>22122</v>
       </c>
@@ -1219,13 +1216,13 @@
         <v>5234</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15">
         <v>60</v>
@@ -1252,7 +1249,7 @@
         <v>4.1366666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>22122</v>
       </c>
@@ -1260,13 +1257,13 @@
         <v>5228</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16">
         <v>60</v>
@@ -1293,7 +1290,7 @@
         <v>44.96</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>22122</v>
       </c>
@@ -1301,13 +1298,13 @@
         <v>5229</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17">
         <v>13.19</v>
@@ -1334,7 +1331,7 @@
         <v>9.4866666666666664</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>22122</v>
       </c>
@@ -1342,13 +1339,13 @@
         <v>5224</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18">
         <v>6.63</v>
@@ -1375,7 +1372,7 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>22122</v>
       </c>
@@ -1383,13 +1380,13 @@
         <v>5226</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19">
         <v>13.71</v>
@@ -1416,7 +1413,7 @@
         <v>42.583333333333336</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>22122</v>
       </c>
@@ -1424,13 +1421,13 @@
         <v>5205</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20">
         <v>60</v>
@@ -1457,7 +1454,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>22122</v>
       </c>
@@ -1465,13 +1462,13 @@
         <v>5206</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21">
         <v>4.21</v>
@@ -1498,7 +1495,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22122</v>
       </c>
@@ -1506,13 +1503,13 @@
         <v>5235</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22">
         <v>5.58</v>
@@ -1539,7 +1536,7 @@
         <v>2.2733333333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22122</v>
       </c>
@@ -1547,13 +1544,13 @@
         <v>5238</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23">
         <v>38.19</v>
@@ -1580,7 +1577,7 @@
         <v>15.773333333333335</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21822</v>
       </c>
@@ -1588,13 +1585,13 @@
         <v>5239</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24">
         <v>13.85</v>
@@ -1621,7 +1618,7 @@
         <v>8.5299999999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21822</v>
       </c>
@@ -1629,13 +1626,13 @@
         <v>5240</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25">
         <v>2.82</v>
@@ -1662,7 +1659,7 @@
         <v>5.3633333333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>21822</v>
       </c>
@@ -1670,13 +1667,13 @@
         <v>5241</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26">
         <v>11.18</v>
@@ -1703,7 +1700,7 @@
         <v>8.6333333333333329</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21822</v>
       </c>
@@ -1711,13 +1708,13 @@
         <v>5242</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F27">
         <v>11.89</v>
@@ -1744,7 +1741,7 @@
         <v>3.3866666666666667</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>21822</v>
       </c>
@@ -1752,13 +1749,13 @@
         <v>5243</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28">
         <v>54.02</v>
@@ -1785,7 +1782,7 @@
         <v>6.8066666666666675</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>21822</v>
       </c>
@@ -1793,13 +1790,13 @@
         <v>5245</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
         <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29">
         <v>3.13</v>
@@ -1826,7 +1823,7 @@
         <v>3.7399999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>21822</v>
       </c>
@@ -1834,13 +1831,13 @@
         <v>5246</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30">
         <v>27.27</v>
@@ -1867,7 +1864,7 @@
         <v>6.0966666666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>21822</v>
       </c>
@@ -1875,13 +1872,13 @@
         <v>5220</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31">
         <v>26.21</v>
@@ -1908,7 +1905,7 @@
         <v>24.01</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>21822</v>
       </c>
@@ -1916,13 +1913,13 @@
         <v>5221</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32">
         <v>60</v>
@@ -1949,7 +1946,7 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>21822</v>
       </c>
@@ -1957,13 +1954,13 @@
         <v>5222</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33">
         <v>29.21</v>
@@ -1990,7 +1987,7 @@
         <v>9.413333333333334</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>21822</v>
       </c>
@@ -1998,13 +1995,13 @@
         <v>5223</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
         <v>21</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F34">
         <v>35.82</v>
@@ -2031,7 +2028,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44717</v>
       </c>
@@ -2039,13 +2036,13 @@
         <v>5328</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" t="s">
         <v>21</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F35">
         <v>17.53</v>
@@ -2072,7 +2069,7 @@
         <v>14.036666666666667</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>44717</v>
       </c>
@@ -2080,13 +2077,13 @@
         <v>5329</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
         <v>21</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F36">
         <v>10.08</v>
@@ -2113,7 +2110,7 @@
         <v>7.16</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>44717</v>
       </c>
@@ -2121,13 +2118,13 @@
         <v>5330</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F37">
         <v>13.59</v>
@@ -2154,7 +2151,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>44717</v>
       </c>
@@ -2162,13 +2159,13 @@
         <v>5331</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F38">
         <v>3.78</v>
@@ -2195,7 +2192,7 @@
         <v>13.826666666666668</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>44717</v>
       </c>
@@ -2203,13 +2200,13 @@
         <v>5316</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F39">
         <v>7.2</v>
@@ -2236,7 +2233,7 @@
         <v>17.253333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>44717</v>
       </c>
@@ -2244,13 +2241,13 @@
         <v>5317</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F40">
         <v>8.5299999999999994</v>
@@ -2277,7 +2274,7 @@
         <v>11.066666666666665</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>44717</v>
       </c>
@@ -2285,13 +2282,13 @@
         <v>5289</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F41">
         <v>10.029999999999999</v>
@@ -2318,7 +2315,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>44717</v>
       </c>
@@ -2326,13 +2323,13 @@
         <v>5290</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F42">
         <v>3.19</v>
@@ -2359,7 +2356,7 @@
         <v>31.183333333333337</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>44717</v>
       </c>
@@ -2367,13 +2364,13 @@
         <v>5292</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F43">
         <v>7.59</v>
@@ -2400,7 +2397,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>44717</v>
       </c>
@@ -2408,13 +2405,13 @@
         <v>5293</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F44">
         <v>6.34</v>
@@ -2441,7 +2438,7 @@
         <v>40.416666666666664</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44717</v>
       </c>
@@ -2449,13 +2446,13 @@
         <v>5312</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
         <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F45">
         <v>5.35</v>
@@ -2482,7 +2479,7 @@
         <v>13.206666666666669</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44717</v>
       </c>
@@ -2490,13 +2487,13 @@
         <v>5313</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D46" t="s">
         <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F46">
         <v>60</v>
@@ -2523,7 +2520,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44717</v>
       </c>
@@ -2531,13 +2528,13 @@
         <v>5314</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F47">
         <v>4.84</v>
@@ -2564,7 +2561,7 @@
         <v>42.37</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44717</v>
       </c>
@@ -2572,13 +2569,13 @@
         <v>5310</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D48" t="s">
         <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F48">
         <v>60</v>
@@ -2605,7 +2602,7 @@
         <v>6.883</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>44717</v>
       </c>
@@ -2613,13 +2610,13 @@
         <v>5311</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D49" t="s">
         <v>21</v>
       </c>
       <c r="E49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F49">
         <v>11.63</v>
@@ -2646,73 +2643,73 @@
         <v>19.72666666666667</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
     </row>
   </sheetData>
@@ -2725,21 +2722,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB76AF-E215-4F64-BFE2-860AA2B92005}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1">
         <v>60</v>
@@ -2766,15 +2763,15 @@
         <v>4.1366666666666667</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -2801,15 +2798,15 @@
         <v>44.96</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>13.19</v>
@@ -2836,15 +2833,15 @@
         <v>9.4866666666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>13.71</v>
@@ -2871,15 +2868,15 @@
         <v>42.583333333333336</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>60</v>
@@ -2906,15 +2903,15 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>54.02</v>
@@ -2941,15 +2938,15 @@
         <v>6.8066666666666675</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>26.21</v>
@@ -2976,15 +2973,15 @@
         <v>24.01</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>60</v>
@@ -3011,15 +3008,15 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>35.82</v>
@@ -3046,15 +3043,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>10.58</v>
@@ -3081,15 +3078,15 @@
         <v>6.8500000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>16.329999999999998</v>
@@ -3116,15 +3113,15 @@
         <v>12.973333333333334</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>12.71</v>
@@ -3151,15 +3148,15 @@
         <v>13.74</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>5.45</v>
@@ -3186,15 +3183,15 @@
         <v>14.443333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14">
         <v>14.7</v>
@@ -3221,15 +3218,15 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>17.53</v>
@@ -3256,15 +3253,15 @@
         <v>14.036666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>10.08</v>
@@ -3291,15 +3288,15 @@
         <v>7.16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17">
         <v>13.59</v>
@@ -3326,15 +3323,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>5.35</v>
@@ -3361,15 +3358,15 @@
         <v>13.206666666666669</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>60</v>
@@ -3396,15 +3393,15 @@
         <v>6.883</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20">
         <v>11.63</v>
@@ -3431,15 +3428,15 @@
         <v>19.72666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21">
         <v>6.63</v>
@@ -3466,15 +3463,15 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22">
         <v>4.21</v>
@@ -3501,15 +3498,15 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23">
         <v>5.58</v>
@@ -3536,15 +3533,15 @@
         <v>2.2733333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24">
         <v>38.19</v>
@@ -3571,15 +3568,15 @@
         <v>15.773333333333335</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25">
         <v>13.85</v>
@@ -3606,15 +3603,15 @@
         <v>8.5299999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26">
         <v>2.82</v>
@@ -3641,15 +3638,15 @@
         <v>5.3633333333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27">
         <v>29.21</v>
@@ -3676,15 +3673,15 @@
         <v>9.413333333333334</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28">
         <v>7.2</v>
@@ -3711,15 +3708,15 @@
         <v>17.253333333333334</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29">
         <v>8.5299999999999994</v>
@@ -3746,15 +3743,15 @@
         <v>11.066666666666665</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30">
         <v>10.029999999999999</v>
@@ -3781,15 +3778,15 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>3.19</v>
@@ -3816,15 +3813,15 @@
         <v>31.183333333333337</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32">
         <v>7.59</v>
@@ -3851,15 +3848,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33">
         <v>6.34</v>
@@ -3886,15 +3883,15 @@
         <v>40.416666666666664</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34">
         <v>7.38</v>
@@ -3921,15 +3918,15 @@
         <v>9.0533333333333328</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35">
         <v>7.33</v>
@@ -3956,15 +3953,15 @@
         <v>4.3299999999999992</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36">
         <v>8.32</v>
@@ -3991,15 +3988,15 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37">
         <v>7.28</v>
@@ -4026,15 +4023,15 @@
         <v>6.5766666666666671</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38">
         <v>3.7</v>
@@ -4061,15 +4058,15 @@
         <v>7.5333333333333323</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39">
         <v>9.57</v>
@@ -4096,15 +4093,15 @@
         <v>4.1499999999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40">
         <v>22.96</v>
@@ -4131,15 +4128,15 @@
         <v>9.0233333333333334</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41">
         <v>19.399999999999999</v>
@@ -4166,15 +4163,15 @@
         <v>3.4633333333333334</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42">
         <v>11.18</v>
@@ -4201,15 +4198,15 @@
         <v>8.6333333333333329</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43">
         <v>11.89</v>
@@ -4236,15 +4233,15 @@
         <v>3.3866666666666667</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D44">
         <v>3.13</v>
@@ -4271,15 +4268,15 @@
         <v>3.7399999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45">
         <v>27.27</v>
@@ -4306,15 +4303,15 @@
         <v>6.0966666666666667</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46">
         <v>3.78</v>
@@ -4341,15 +4338,15 @@
         <v>13.826666666666668</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47">
         <v>60</v>
@@ -4376,15 +4373,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
       </c>
       <c r="C48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48">
         <v>4.84</v>

</xml_diff>